<commit_message>
reconfigure tc 002, 005, 006, 007, 008 and reorganize data files
</commit_message>
<xml_diff>
--- a/Data Files/AOS0001.xlsx
+++ b/Data Files/AOS0001.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Katalon Studio\AOS-Mobile\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3257C17-36D7-471F-B376-767F0D1AB656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723B2CCD-3FD6-4EF3-AFA2-9C5DA94B63C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TC-006" sheetId="3" r:id="rId1"/>
-    <sheet name="TC-005" sheetId="2" r:id="rId2"/>
-    <sheet name="TC-002" sheetId="1" r:id="rId3"/>
+    <sheet name="LIST_REGISTERED_ACCOUNT" sheetId="4" r:id="rId1"/>
+    <sheet name="LIST_UNREGISTERED_ACCOUNT" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
   <si>
     <t>USERNAME</t>
   </si>
@@ -53,24 +52,6 @@
     <t>!Reaganwa47</t>
   </si>
   <si>
-    <t>asusexpertbook</t>
-  </si>
-  <si>
-    <t>!Asus123</t>
-  </si>
-  <si>
-    <t>bankbni</t>
-  </si>
-  <si>
-    <t>!BankBNI123</t>
-  </si>
-  <si>
-    <t>katalonstudio</t>
-  </si>
-  <si>
-    <t>#!Katalon123</t>
-  </si>
-  <si>
     <t>EMAIL</t>
   </si>
   <si>
@@ -81,6 +62,255 @@
   </si>
   <si>
     <t>wallace.reagan@mrrworks.com</t>
+  </si>
+  <si>
+    <t>CONFIRM_PASSWORD</t>
+  </si>
+  <si>
+    <t>FIRST_NAME</t>
+  </si>
+  <si>
+    <t>LAST_NAME</t>
+  </si>
+  <si>
+    <t>PHONE_NUMBER</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>STATE/PROVINCE/REGION</t>
+  </si>
+  <si>
+    <t>POSTAL_CODE</t>
+  </si>
+  <si>
+    <t>Rafly</t>
+  </si>
+  <si>
+    <t>SQA</t>
+  </si>
+  <si>
+    <t>081295940847</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Bekasi</t>
+  </si>
+  <si>
+    <t>Tambun</t>
+  </si>
+  <si>
+    <t>West Java</t>
+  </si>
+  <si>
+    <t>Chaya</t>
+  </si>
+  <si>
+    <t>Sampson</t>
+  </si>
+  <si>
+    <t>081253444384</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Reagan</t>
+  </si>
+  <si>
+    <t>Wallace</t>
+  </si>
+  <si>
+    <t>081220075502</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>thompson.daisy@mrrworks.com</t>
+  </si>
+  <si>
+    <t>!Daisyth52</t>
+  </si>
+  <si>
+    <t>Daisy</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>081267456418</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>walter.mckenna@mrrworks.com</t>
+  </si>
+  <si>
+    <t>!Mckennawa54</t>
+  </si>
+  <si>
+    <t>Mckenna</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>081274783582</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>donaldson.jayden@mrrworks.com</t>
+  </si>
+  <si>
+    <t>!Jaydendo83</t>
+  </si>
+  <si>
+    <t>Jayden</t>
+  </si>
+  <si>
+    <t>Donaldson</t>
+  </si>
+  <si>
+    <t>081240382201</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>villegas.libby@mrrworks.com</t>
+  </si>
+  <si>
+    <t>!Libbyvi57</t>
+  </si>
+  <si>
+    <t>Libby</t>
+  </si>
+  <si>
+    <t>Villegas</t>
+  </si>
+  <si>
+    <t>081212697000</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>patrick.laylah@mrrworks.com</t>
+  </si>
+  <si>
+    <t>!Laylahpa44</t>
+  </si>
+  <si>
+    <t>Laylah</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>081296961284</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Fatima</t>
+  </si>
+  <si>
+    <t>Mosley</t>
+  </si>
+  <si>
+    <t>Josie</t>
+  </si>
+  <si>
+    <t>Noah</t>
+  </si>
+  <si>
+    <t>Fiona</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Gonzales</t>
+  </si>
+  <si>
+    <t>Marshall</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>081216361284</t>
+  </si>
+  <si>
+    <t>089292366734</t>
+  </si>
+  <si>
+    <t>daisy.tho</t>
+  </si>
+  <si>
+    <t>mckenna.wal</t>
+  </si>
+  <si>
+    <t>jayden.don</t>
+  </si>
+  <si>
+    <t>libby.vil</t>
+  </si>
+  <si>
+    <t>laylah.pat</t>
+  </si>
+  <si>
+    <t>fatima.mos</t>
+  </si>
+  <si>
+    <t>Fatima.Mosley@mrr.works</t>
+  </si>
+  <si>
+    <t>#Fatimamo92</t>
+  </si>
+  <si>
+    <t>fiona.tay</t>
+  </si>
+  <si>
+    <t>Fiona.Taylor@mrr.works</t>
+  </si>
+  <si>
+    <t>#Fionata92</t>
+  </si>
+  <si>
+    <t>noah.gon</t>
+  </si>
+  <si>
+    <t>Noah.Gonzales@mrr.works</t>
+  </si>
+  <si>
+    <t>#Noahgo92</t>
+  </si>
+  <si>
+    <t>josie.mar</t>
+  </si>
+  <si>
+    <t>Josie.Marshall@mrr.works</t>
+  </si>
+  <si>
+    <t>#Josiema92</t>
   </si>
 </sst>
 </file>
@@ -116,8 +346,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,49 +628,179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4253B306-E514-4135-B660-773667DBD5D2}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DDB02F2-58A6-439A-A588-B7115399D402}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="A1:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4">
+        <v>17510</v>
       </c>
     </row>
   </sheetData>
@@ -448,100 +809,407 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D72F37-0EE0-455D-8E85-4BFE386B4D45}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1115166C-23BE-4FA2-9C22-737897B35AE2}">
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9">
+        <v>17510</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10">
+        <v>17510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>